<commit_message>
Autocompletar que consulta de la base de datos, agregada columna estatus_valido a insert, y ajustado a documento excel descargable
</commit_message>
<xml_diff>
--- a/registro.xlsx
+++ b/registro.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
   <si>
     <t>DATOS PERSONALES DE LA PAREJA CONCURSANTE</t>
   </si>
@@ -53,6 +53,9 @@
     <t>DOCUMENTOS PRESENTADOS PARTICIPANTE</t>
   </si>
   <si>
+    <t xml:space="preserve">CURP A.N. INE Foto </t>
+  </si>
+  <si>
     <t>DOCUMENTOS PRESENTADOS PAREJA</t>
   </si>
   <si>
@@ -60,6 +63,9 @@
   </si>
   <si>
     <t>NOMBRE COMPLETO DEL PADRE Y/O TUTOR DEL PARTICIPANTE:</t>
+  </si>
+  <si>
+    <t>Paco</t>
   </si>
   <si>
     <t>TELEFONO DE CONTACTO:</t>
@@ -127,19 +133,19 @@
       <i val="0"/>
       <strike val="0"/>
       <u val="none"/>
-      <sz val="13"/>
+      <sz val="95"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
+      <name val="Arial Black"/>
     </font>
     <font>
       <b val="0"/>
       <i val="0"/>
       <strike val="0"/>
       <u val="none"/>
-      <sz val="95"/>
+      <sz val="13"/>
       <color rgb="FF000000"/>
-      <name val="Arial Black"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -220,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
@@ -230,45 +236,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection locked="false"/>
     </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection locked="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="4" quotePrefix="1" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection locked="false"/>
-    </xf>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection locked="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0" applyProtection="true">
-      <protection locked="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
@@ -280,18 +247,62 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection locked="false"/>
     </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" quotePrefix="1" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <protection locked="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <protection locked="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="0" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="0" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="0" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <protection locked="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="2" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <protection locked="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="3" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <protection locked="false"/>
+    </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="4" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection locked="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -678,8 +689,8 @@
   </sheetPr>
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1" topLeftCell="A22">
-      <selection activeCell="D30" sqref="D30:H35"/>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1" topLeftCell="A16">
+      <selection activeCell="E24" sqref="E24:J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -690,151 +701,151 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10">
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:10" customHeight="1" ht="17.25">
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
     </row>
     <row r="13" spans="1:10" customHeight="1" ht="17.25">
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:10" customHeight="1" ht="30">
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="16" t="s">
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
       <c r="I14" s="1" t="s">
         <v>3</v>
       </c>
@@ -843,17 +854,17 @@
       </c>
     </row>
     <row r="15" spans="1:10" customHeight="1" ht="30">
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="16" t="s">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
       <c r="I15" s="1" t="s">
         <v>3</v>
       </c>
@@ -862,284 +873,271 @@
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="16">
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="20">
         <v>123456789</v>
       </c>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="19"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10" customHeight="1" ht="30">
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="16" t="s">
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="19"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10" customHeight="1" ht="30.75">
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
     </row>
     <row r="19" spans="1:10" customHeight="1" ht="30.75">
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
     </row>
     <row r="21" spans="1:10" customHeight="1" ht="17.25">
-      <c r="B21" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
+      <c r="B21" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
     </row>
     <row r="22" spans="1:10" customHeight="1" ht="17.25">
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="B23" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
+      <c r="B23" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
     </row>
     <row r="24" spans="1:10">
-      <c r="B24" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="13">
+      <c r="B24" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="19">
         <v>123456789</v>
       </c>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
     </row>
     <row r="26" spans="1:10" customHeight="1" ht="17.25">
-      <c r="B26" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
+      <c r="B26" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
     </row>
     <row r="27" spans="1:10" customHeight="1" ht="17.25">
-      <c r="B27" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="7"/>
+      <c r="B27" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="B28" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
+      <c r="B28" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" customHeight="1" ht="17.25">
-      <c r="B29" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29" s="9"/>
-      <c r="D29" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="J29" s="9"/>
+      <c r="B29" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" s="12"/>
+      <c r="D29" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="J29" s="12"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="10">
-        <v>144</v>
-      </c>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="13">
+        <v>135</v>
+      </c>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
     </row>
     <row r="31" spans="1:10">
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="9"/>
-      <c r="J31" s="9"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
     </row>
     <row r="32" spans="1:10">
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="9"/>
-      <c r="J32" s="9"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="12"/>
     </row>
     <row r="33" spans="1:10">
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="9"/>
-      <c r="J33" s="9"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
     </row>
     <row r="34" spans="1:10">
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="9"/>
-      <c r="J34" s="9"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
     </row>
     <row r="35" spans="1:10">
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="9"/>
-      <c r="J35" s="9"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
     </row>
   </sheetData>
   <mergeCells>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="B2:J4"/>
-    <mergeCell ref="B5:J10"/>
-    <mergeCell ref="B11:J11"/>
-    <mergeCell ref="B12:J12"/>
-    <mergeCell ref="B13:J13"/>
-    <mergeCell ref="B21:J21"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E16:J16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E17:J17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:J18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E19:J19"/>
-    <mergeCell ref="B20:J20"/>
     <mergeCell ref="B29:C35"/>
     <mergeCell ref="D29:H29"/>
     <mergeCell ref="I29:J35"/>
@@ -1155,6 +1153,25 @@
     <mergeCell ref="E27:J27"/>
     <mergeCell ref="B28:D28"/>
     <mergeCell ref="E28:J28"/>
+    <mergeCell ref="B21:J21"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:J16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:J17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:J18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E19:J19"/>
+    <mergeCell ref="B20:J20"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="B2:J4"/>
+    <mergeCell ref="B5:J10"/>
+    <mergeCell ref="B11:J11"/>
+    <mergeCell ref="B12:J12"/>
+    <mergeCell ref="B13:J13"/>
   </mergeCells>
   <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" sqref="E28:J28">

</xml_diff>